<commit_message>
Scripting DPLKINV003-004 and DPLKINV003-006 until DPLKINV003-008
</commit_message>
<xml_diff>
--- a/DPLKINV003-005 - Fixed Income - Upload Harga Pasar/Report/Report/Default.xlsx
+++ b/DPLKINV003-005 - Fixed Income - Upload Harga Pasar/Report/Report/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="DPLKINV003-001-Investasi-Fixed" sheetId="2" r:id="rId2"/>
+    <sheet name="DPLKINV003-005-Investasi-Fixed" sheetId="2" r:id="rId2"/>
     <sheet name="TEMPORARY" sheetId="3" r:id="rId3"/>
     <sheet name="DPLKDBConfig" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -37,7 +37,7 @@
     <t>C:\Program Files\HeidiSQL</t>
   </si>
   <si>
-    <t>DPLKINV003-001</t>
+    <t>DPLKINV003-005</t>
   </si>
   <si>
     <t>VALUTA</t>
@@ -103,9 +103,6 @@
     <t>Fixed Income</t>
   </si>
   <si>
-    <t>01012023HargaPasarFixedIncome.xlsx</t>
-  </si>
-  <si>
     <t>QUERY_SETUP_PORTOFOLIO</t>
   </si>
   <si>
@@ -149,174 +146,177 @@
   </si>
   <si>
     <t>TESTER2</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY2</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>BROWSER_VERSION</t>
+  </si>
+  <si>
+    <t>COVER_TITLE</t>
+  </si>
+  <si>
+    <t>Regression Test</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT_MANAGER</t>
+  </si>
+  <si>
+    <t>Investasi</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>107.0.5304.107 (Official Build) (64-bit)</t>
+  </si>
+  <si>
+    <t>BROWSER_ICONS</t>
+  </si>
+  <si>
+    <t>filezilla</t>
+  </si>
+  <si>
+    <t>Upload harga pasar Reksadana - Fixed Income dapat dilakukan dengan baik</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>MAIN_SIDEBAR</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>select * from dbo.inv_ms_portofolio where porto_id = '&lt;OBJECT_1&gt;';</t>
+  </si>
+  <si>
+    <t>DATABASE_2</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>http://192.168.168.111/</t>
+  </si>
+  <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
+    <t>Automation Team</t>
+  </si>
+  <si>
+    <t>TESTING_GROUPHEAD</t>
+  </si>
+  <si>
+    <t>PROGRAM1</t>
+  </si>
+  <si>
+    <t>QUERY3</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>Automation Tester 1</t>
+  </si>
+  <si>
+    <t>REQUIREMENT_MANAGER</t>
+  </si>
+  <si>
+    <t>C:\Program Files\FileZilla FTP Client</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>Investasi - Fixed Income</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY3</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>BROWSER</t>
+  </si>
+  <si>
+    <t>HEADER_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>PROGRAM_PATH1</t>
+  </si>
+  <si>
+    <t>Entry Harga Pasar</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Project Code</t>
+  </si>
+  <si>
+    <t>heidisql</t>
+  </si>
+  <si>
+    <t>SCENARIO_DESC</t>
+  </si>
+  <si>
+    <t>SIDEBAR_SUBMENU</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>iexplore</t>
+  </si>
+  <si>
+    <t>DPLK - Regression Test</t>
+  </si>
+  <si>
+    <t>PROGRAM2</t>
+  </si>
+  <si>
+    <t>EXPECTED_RESULT</t>
   </si>
   <si>
     <t>Username : 32382;
 Password : bni1234;
-Tgl. Market : 01/01/2023;
-File Excel : 01012023HargaPasarFixedIncome.xlsx</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY2</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>AQ</t>
-  </si>
-  <si>
-    <t>BROWSER_VERSION</t>
-  </si>
-  <si>
-    <t>COVER_TITLE</t>
-  </si>
-  <si>
-    <t>Regression Test</t>
-  </si>
-  <si>
-    <t>DEVELOPMENT_MANAGER</t>
-  </si>
-  <si>
-    <t>Investasi</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>107.0.5304.107 (Official Build) (64-bit)</t>
-  </si>
-  <si>
-    <t>BROWSER_ICONS</t>
-  </si>
-  <si>
-    <t>filezilla</t>
-  </si>
-  <si>
-    <t>Upload harga pasar Reksadana - Fixed Income dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>PREPARATION</t>
-  </si>
-  <si>
-    <t>MAIN_SIDEBAR</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>select * from dbo.inv_ms_portofolio where porto_id = '&lt;OBJECT_1&gt;';</t>
-  </si>
-  <si>
-    <t>DATABASE_2</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>AUTHOR</t>
-  </si>
-  <si>
-    <t>Automation Team</t>
-  </si>
-  <si>
-    <t>TESTING_GROUPHEAD</t>
-  </si>
-  <si>
-    <t>PROGRAM1</t>
-  </si>
-  <si>
-    <t>QUERY3</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
-    <t>AJ</t>
-  </si>
-  <si>
-    <t>http://192.168.168.107/</t>
-  </si>
-  <si>
-    <t>Automation Tester 1</t>
-  </si>
-  <si>
-    <t>REQUIREMENT_MANAGER</t>
-  </si>
-  <si>
-    <t>C:\Program Files\FileZilla FTP Client</t>
-  </si>
-  <si>
-    <t>TC_ID</t>
-  </si>
-  <si>
-    <t>Investasi - Fixed Income</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY3</t>
-  </si>
-  <si>
-    <t>AN</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>BROWSER</t>
-  </si>
-  <si>
-    <t>HEADER_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>PROGRAM_PATH1</t>
-  </si>
-  <si>
-    <t>Entry Harga Pasar</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Project Code</t>
-  </si>
-  <si>
-    <t>heidisql</t>
-  </si>
-  <si>
-    <t>SCENARIO_DESC</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>iexplore</t>
-  </si>
-  <si>
-    <t>DPLK - Regression Test</t>
-  </si>
-  <si>
-    <t>PROGRAM2</t>
-  </si>
-  <si>
-    <t>EXPECTED_RESULT</t>
+Tgl. Market : 05/01/2023;
+File Excel : 05012023HargaPasarFixedIncome.xlsx</t>
+  </si>
+  <si>
+    <t>05012023HargaPasarFixedIncome.xlsx</t>
   </si>
   <si>
     <t>M</t>
@@ -633,62 +633,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1027,25 +1027,25 @@
         <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
         <v>113</v>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" t="s">
         <v>114</v>
@@ -1066,40 +1066,40 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
         <v>105</v>
       </c>
       <c r="Q1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T1" t="s">
         <v>24</v>
       </c>
       <c r="U1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W1" t="s">
         <v>4</v>
       </c>
       <c r="X1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y1" t="s">
         <v>2</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -1107,41 +1107,41 @@
         <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>74</v>
+        <v>54</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>104</v>
@@ -1152,19 +1152,19 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="21"/>
+        <v>75</v>
+      </c>
+      <c r="Z2" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1185,29 +1185,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.078125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.078125" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
@@ -1215,19 +1215,19 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
         <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
         <v>26</v>
@@ -1236,13 +1236,13 @@
         <v>115</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
@@ -1254,10 +1254,10 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q1" t="s">
         <v>107</v>
@@ -1266,10 +1266,10 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="U1" t="s">
         <v>108</v>
@@ -1286,16 +1286,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="G2" s="4">
         <v>32382</v>
@@ -1304,31 +1304,31 @@
         <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="19">
-        <v>44930</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>28</v>
+      <c r="M2" s="21">
+        <v>44931</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="O2" s="4"/>
-      <c r="P2" s="12"/>
+      <c r="P2" s="15"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-      <c r="V2" s="20"/>
+      <c r="V2" s="18"/>
     </row>
     <row r="3">
       <c r="A3" s="2"/>
@@ -1340,19 +1340,19 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="16"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="4"/>
       <c r="N3" s="2"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="12"/>
+      <c r="P3" s="15"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="18"/>
+      <c r="V3" s="24"/>
     </row>
     <row r="4" ht="15">
       <c r="A4" s="2"/>
@@ -1364,19 +1364,19 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="22"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="4"/>
       <c r="N4" s="5"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="18"/>
+      <c r="V4" s="24"/>
     </row>
     <row r="5" ht="15">
       <c r="A5" s="2"/>
@@ -1388,23 +1388,23 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="22"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="15"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="18"/>
+      <c r="V5" s="24"/>
     </row>
     <row r="6" ht="15">
       <c r="A6" s="2"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1424,11 +1424,11 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="18"/>
+      <c r="V6" s="24"/>
     </row>
     <row r="7" ht="15">
       <c r="A7" s="2"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1448,7 +1448,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="18"/>
+      <c r="V7" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1485,54 +1485,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="9.078125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.140625" style="16" customWidth="1"/>
-    <col min="13" max="14" width="61" style="16" customWidth="1"/>
-    <col min="15" max="15" width="47" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="103.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="61" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="51" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="49.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="59.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="53.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="56.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="51.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="57.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="35.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.078125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.078125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.140625" style="14" customWidth="1"/>
+    <col min="13" max="14" width="61" style="14" customWidth="1"/>
+    <col min="15" max="15" width="47" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="103.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="69.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="61" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="63.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="51" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="49.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="59.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="53.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="56.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="57.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="58.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="62.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="51.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="57.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="53.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="58.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.078125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -1544,28 +1544,28 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" t="s">
-        <v>71</v>
       </c>
       <c r="M1" t="s">
         <v>99</v>
@@ -1574,10 +1574,10 @@
         <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q1" t="s">
         <v>107</v>
@@ -1586,10 +1586,10 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="U1" t="s">
         <v>108</v>
@@ -1598,34 +1598,34 @@
         <v>17</v>
       </c>
       <c r="W1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y1" t="s">
         <v>117</v>
       </c>
       <c r="Z1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AB1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AD1" t="s">
         <v>9</v>
       </c>
       <c r="AE1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG1" t="s">
         <v>100</v>
@@ -1634,10 +1634,10 @@
         <v>10</v>
       </c>
       <c r="AI1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AJ1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AK1" t="s">
         <v>101</v>
@@ -1646,10 +1646,10 @@
         <v>11</v>
       </c>
       <c r="AM1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AN1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AO1" t="s">
         <v>110</v>
@@ -1658,10 +1658,10 @@
         <v>21</v>
       </c>
       <c r="AQ1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AR1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AS1" t="s">
         <v>111</v>
@@ -1672,12 +1672,12 @@
     </row>
     <row r="2" ht="36">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="19">
         <v>192168132154</v>
       </c>
       <c r="D2" s="4" t="str">
@@ -1685,9 +1685,9 @@
         <v>Verifikasi Database DPLK</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2"/>
@@ -1729,7 +1729,7 @@
       <c r="AQ2" s="8"/>
       <c r="AR2" s="8"/>
       <c r="AS2" s="8"/>
-      <c r="AT2" s="24"/>
+      <c r="AT2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>